<commit_message>
The speed will become faster act game continue
</commit_message>
<xml_diff>
--- a/Assets/Excel/MarryCondition.xlsx
+++ b/Assets/Excel/MarryCondition.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="25600" windowHeight="12210"/>
+    <workbookView windowWidth="19350" windowHeight="11460"/>
   </bookViews>
   <sheets>
     <sheet name="MarryCondition" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="38">
   <si>
     <t>//dontCare</t>
   </si>
@@ -23,6 +23,9 @@
   </si>
   <si>
     <t>numMarriage</t>
+  </si>
+  <si>
+    <t>timeOfYear</t>
   </si>
   <si>
     <t>ageMinM</t>
@@ -1128,36 +1131,37 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:AH23"/>
+  <dimension ref="A1:AI23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
       <selection/>
-      <selection pane="topRight" activeCell="Y28" sqref="Y28"/>
+      <selection pane="topRight" activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
   <cols>
     <col min="1" max="1" width="10.9090909090909" customWidth="1"/>
     <col min="2" max="2" width="12.4545454545455" customWidth="1"/>
-    <col min="3" max="3" width="8" customWidth="1"/>
-    <col min="4" max="4" width="8.72727272727273" customWidth="1"/>
-    <col min="5" max="5" width="8" customWidth="1"/>
-    <col min="6" max="6" width="8.72727272727273" customWidth="1"/>
-    <col min="7" max="7" width="6.45454545454545" customWidth="1"/>
-    <col min="8" max="8" width="6.63636363636364" customWidth="1"/>
-    <col min="9" max="11" width="6.90909090909091" customWidth="1"/>
-    <col min="12" max="12" width="6.45454545454545" customWidth="1"/>
-    <col min="13" max="13" width="12.2" customWidth="1"/>
-    <col min="14" max="14" width="6.45454545454545" customWidth="1"/>
-    <col min="15" max="15" width="6.63636363636364" customWidth="1"/>
-    <col min="16" max="18" width="6.90909090909091" customWidth="1"/>
-    <col min="19" max="19" width="6.45454545454545" customWidth="1"/>
-    <col min="20" max="20" width="12.2" customWidth="1"/>
-    <col min="21" max="26" width="9.54545454545454" customWidth="1"/>
-    <col min="27" max="27" width="15.0545454545455" customWidth="1"/>
-    <col min="28" max="33" width="9.54545454545454" customWidth="1"/>
-    <col min="34" max="34" width="15.0545454545455" customWidth="1"/>
+    <col min="3" max="3" width="11.5545454545455" customWidth="1"/>
+    <col min="4" max="4" width="8" customWidth="1"/>
+    <col min="5" max="5" width="8.72727272727273" customWidth="1"/>
+    <col min="6" max="6" width="8" customWidth="1"/>
+    <col min="7" max="7" width="8.72727272727273" customWidth="1"/>
+    <col min="8" max="8" width="6.45454545454545" customWidth="1"/>
+    <col min="9" max="9" width="6.63636363636364" customWidth="1"/>
+    <col min="10" max="12" width="6.90909090909091" customWidth="1"/>
+    <col min="13" max="13" width="6.45454545454545" customWidth="1"/>
+    <col min="14" max="14" width="12.2" customWidth="1"/>
+    <col min="15" max="15" width="6.45454545454545" customWidth="1"/>
+    <col min="16" max="16" width="6.63636363636364" customWidth="1"/>
+    <col min="17" max="19" width="6.90909090909091" customWidth="1"/>
+    <col min="20" max="20" width="6.45454545454545" customWidth="1"/>
+    <col min="21" max="21" width="12.2" customWidth="1"/>
+    <col min="22" max="27" width="9.54545454545454" customWidth="1"/>
+    <col min="28" max="28" width="15.0545454545455" customWidth="1"/>
+    <col min="29" max="34" width="9.54545454545454" customWidth="1"/>
+    <col min="35" max="35" width="15.0545454545455" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -1165,26 +1169,26 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:34">
+    <row r="2" spans="1:35">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>5</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="3" t="s">
         <v>7</v>
       </c>
       <c r="H2" s="4" t="s">
@@ -1202,10 +1206,10 @@
       <c r="L2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="M2" s="5" t="s">
+      <c r="M2" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="N2" s="6" t="s">
+      <c r="N2" s="5" t="s">
         <v>14</v>
       </c>
       <c r="O2" s="6" t="s">
@@ -1223,10 +1227,10 @@
       <c r="S2" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="T2" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="U2" s="4" t="s">
+      <c r="T2" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="U2" s="5" t="s">
         <v>21</v>
       </c>
       <c r="V2" s="4" t="s">
@@ -1244,10 +1248,10 @@
       <c r="Z2" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="AA2" s="5" t="s">
+      <c r="AA2" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="AB2" s="6" t="s">
+      <c r="AB2" s="5" t="s">
         <v>28</v>
       </c>
       <c r="AC2" s="6" t="s">
@@ -1265,115 +1269,121 @@
       <c r="AG2" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="AH2" s="5" t="s">
+      <c r="AH2" s="6" t="s">
         <v>34</v>
       </c>
+      <c r="AI2" s="5" t="s">
+        <v>35</v>
+      </c>
     </row>
-    <row r="3" spans="1:34">
+    <row r="3" spans="1:35">
       <c r="A3" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>36</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>35</v>
+        <v>36</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>36</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="M3" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="N3" s="6" t="s">
-        <v>35</v>
+      <c r="M3" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="N3" s="5" t="s">
+        <v>37</v>
       </c>
       <c r="O3" s="6" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="P3" s="6" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="Q3" s="6" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="R3" s="6" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="S3" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="T3" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="U3" s="4" t="s">
-        <v>35</v>
+      <c r="T3" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="U3" s="5" t="s">
+        <v>37</v>
       </c>
       <c r="V3" s="4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="W3" s="4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="X3" s="4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="Y3" s="4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="Z3" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="AA3" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="AB3" s="6" t="s">
-        <v>35</v>
+      <c r="AA3" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB3" s="5" t="s">
+        <v>37</v>
       </c>
       <c r="AC3" s="6" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="AD3" s="6" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="AE3" s="6" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="AF3" s="6" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="AG3" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="AH3" s="5" t="s">
         <v>36</v>
       </c>
+      <c r="AH3" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="AI3" s="5" t="s">
+        <v>37</v>
+      </c>
     </row>
-    <row r="4" spans="1:34">
+    <row r="4" spans="1:35">
       <c r="A4">
         <v>1001</v>
       </c>
@@ -1381,26 +1391,26 @@
         <v>0</v>
       </c>
       <c r="C4">
+        <v>1.6</v>
+      </c>
+      <c r="D4">
         <v>18</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>50</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>18</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>38</v>
       </c>
-      <c r="G4">
-        <v>10</v>
-      </c>
       <c r="H4">
+        <v>10</v>
+      </c>
+      <c r="I4">
         <v>5</v>
       </c>
-      <c r="I4">
-        <v>0</v>
-      </c>
       <c r="J4">
         <v>0</v>
       </c>
@@ -1411,14 +1421,14 @@
         <v>0</v>
       </c>
       <c r="M4">
-        <f>(G4*0+H4*1+I4*2+J4*3+K4*4+L4*5)/(G4+H4+I4+J4+K4+L4)</f>
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <f>(H4*0+I4*1+J4*2+K4*3+L4*4+M4*5)/(H4+I4+J4+K4+L4+M4)</f>
         <v>0.333333333333333</v>
       </c>
-      <c r="N4">
-        <v>15</v>
-      </c>
       <c r="O4">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="P4">
         <v>0</v>
@@ -1433,14 +1443,14 @@
         <v>0</v>
       </c>
       <c r="T4">
-        <f t="shared" ref="T4:T18" si="0">(N4*0+O4*1+P4*2+Q4*3+R4*4+S4*5)/(N4+O4+P4+Q4+R4+S4)</f>
         <v>0</v>
       </c>
       <c r="U4">
-        <v>10</v>
+        <f t="shared" ref="U4:U18" si="0">(O4*0+P4*1+Q4*2+R4*3+S4*4+T4*5)/(O4+P4+Q4+R4+S4+T4)</f>
+        <v>0</v>
       </c>
       <c r="V4">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="W4">
         <v>0</v>
@@ -1455,14 +1465,14 @@
         <v>0</v>
       </c>
       <c r="AA4">
-        <f t="shared" ref="AA4:AA23" si="1">(U4*0+V4*1+W4*2+X4*3+Y4*4+Z4*5)/(U4+V4+W4+X4+Y4+Z4)</f>
         <v>0</v>
       </c>
       <c r="AB4">
-        <v>15</v>
+        <f t="shared" ref="AB4:AB23" si="1">(V4*0+W4*1+X4*2+Y4*3+Z4*4+AA4*5)/(V4+W4+X4+Y4+Z4+AA4)</f>
+        <v>0</v>
       </c>
       <c r="AC4">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="AD4">
         <v>0</v>
@@ -1477,11 +1487,14 @@
         <v>0</v>
       </c>
       <c r="AH4">
-        <f t="shared" ref="AH4:AH23" si="2">(AB4*0+AC4*1+AD4*2+AE4*3+AF4*4+AG4*5)/(AB4+AC4+AD4+AE4+AF4+AG4)</f>
+        <v>0</v>
+      </c>
+      <c r="AI4">
+        <f t="shared" ref="AI4:AI23" si="2">(AC4*0+AD4*1+AE4*2+AF4*3+AG4*4+AH4*5)/(AC4+AD4+AE4+AF4+AG4+AH4)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:34">
+    <row r="5" spans="1:35">
       <c r="A5">
         <v>1002</v>
       </c>
@@ -1489,25 +1502,25 @@
         <v>1</v>
       </c>
       <c r="C5">
+        <v>1.6</v>
+      </c>
+      <c r="D5">
         <v>18</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>49</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>18</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>37</v>
       </c>
-      <c r="G5">
-        <v>10</v>
-      </c>
       <c r="H5">
         <v>10</v>
       </c>
       <c r="I5">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="J5">
         <v>0</v>
@@ -1519,18 +1532,18 @@
         <v>0</v>
       </c>
       <c r="M5">
-        <f t="shared" ref="M5:M23" si="3">(G5*0+H5*1+I5*2+J5*3+K5*4+L5*5)/(G5+H5+I5+J5+K5+L5)</f>
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <f t="shared" ref="N5:N23" si="3">(H5*0+I5*1+J5*2+K5*3+L5*4+M5*5)/(H5+I5+J5+K5+L5+M5)</f>
         <v>0.5</v>
       </c>
-      <c r="N5">
-        <v>15</v>
-      </c>
       <c r="O5">
+        <v>15</v>
+      </c>
+      <c r="P5">
         <v>5</v>
       </c>
-      <c r="P5">
-        <v>0</v>
-      </c>
       <c r="Q5">
         <v>0</v>
       </c>
@@ -1541,18 +1554,18 @@
         <v>0</v>
       </c>
       <c r="T5">
+        <v>0</v>
+      </c>
+      <c r="U5">
         <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
-      <c r="U5">
-        <v>10</v>
-      </c>
       <c r="V5">
+        <v>10</v>
+      </c>
+      <c r="W5">
         <v>2</v>
       </c>
-      <c r="W5">
-        <v>0</v>
-      </c>
       <c r="X5">
         <v>0</v>
       </c>
@@ -1563,18 +1576,18 @@
         <v>0</v>
       </c>
       <c r="AA5">
+        <v>0</v>
+      </c>
+      <c r="AB5">
         <f t="shared" si="1"/>
         <v>0.166666666666667</v>
       </c>
-      <c r="AB5">
-        <v>15</v>
-      </c>
       <c r="AC5">
+        <v>15</v>
+      </c>
+      <c r="AD5">
         <v>3</v>
       </c>
-      <c r="AD5">
-        <v>0</v>
-      </c>
       <c r="AE5">
         <v>0</v>
       </c>
@@ -1585,11 +1598,14 @@
         <v>0</v>
       </c>
       <c r="AH5">
+        <v>0</v>
+      </c>
+      <c r="AI5">
         <f t="shared" si="2"/>
         <v>0.166666666666667</v>
       </c>
     </row>
-    <row r="6" spans="1:34">
+    <row r="6" spans="1:35">
       <c r="A6">
         <v>1003</v>
       </c>
@@ -1597,29 +1613,29 @@
         <v>2</v>
       </c>
       <c r="C6">
+        <v>1.6</v>
+      </c>
+      <c r="D6">
         <v>19</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <v>49</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>18</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>37</v>
       </c>
-      <c r="G6">
-        <v>10</v>
-      </c>
       <c r="H6">
         <v>10</v>
       </c>
       <c r="I6">
+        <v>10</v>
+      </c>
+      <c r="J6">
         <v>5</v>
       </c>
-      <c r="J6">
-        <v>0</v>
-      </c>
       <c r="K6">
         <v>0</v>
       </c>
@@ -1627,17 +1643,17 @@
         <v>0</v>
       </c>
       <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6">
         <f t="shared" si="3"/>
         <v>0.8</v>
       </c>
-      <c r="N6">
-        <v>15</v>
-      </c>
       <c r="O6">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="P6">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="Q6">
         <v>0</v>
@@ -1649,18 +1665,18 @@
         <v>0</v>
       </c>
       <c r="T6">
+        <v>0</v>
+      </c>
+      <c r="U6">
         <f t="shared" si="0"/>
         <v>0.4</v>
       </c>
-      <c r="U6">
-        <v>10</v>
-      </c>
       <c r="V6">
+        <v>10</v>
+      </c>
+      <c r="W6">
         <v>5</v>
       </c>
-      <c r="W6">
-        <v>0</v>
-      </c>
       <c r="X6">
         <v>0</v>
       </c>
@@ -1671,18 +1687,18 @@
         <v>0</v>
       </c>
       <c r="AA6">
+        <v>0</v>
+      </c>
+      <c r="AB6">
         <f t="shared" si="1"/>
         <v>0.333333333333333</v>
       </c>
-      <c r="AB6">
-        <v>15</v>
-      </c>
       <c r="AC6">
+        <v>15</v>
+      </c>
+      <c r="AD6">
         <v>6</v>
       </c>
-      <c r="AD6">
-        <v>0</v>
-      </c>
       <c r="AE6">
         <v>0</v>
       </c>
@@ -1693,11 +1709,14 @@
         <v>0</v>
       </c>
       <c r="AH6">
+        <v>0</v>
+      </c>
+      <c r="AI6">
         <f t="shared" si="2"/>
         <v>0.285714285714286</v>
       </c>
     </row>
-    <row r="7" spans="1:34">
+    <row r="7" spans="1:35">
       <c r="A7">
         <v>1004</v>
       </c>
@@ -1705,28 +1724,28 @@
         <v>3</v>
       </c>
       <c r="C7">
+        <v>1.6</v>
+      </c>
+      <c r="D7">
         <v>19</v>
       </c>
-      <c r="D7">
+      <c r="E7">
         <v>48</v>
       </c>
-      <c r="E7">
+      <c r="F7">
         <v>18</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <v>36</v>
       </c>
-      <c r="G7">
-        <v>10</v>
-      </c>
       <c r="H7">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="I7">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="J7">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="K7">
         <v>0</v>
@@ -1735,17 +1754,17 @@
         <v>0</v>
       </c>
       <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="N7">
-        <v>15</v>
-      </c>
       <c r="O7">
         <v>15</v>
       </c>
       <c r="P7">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="Q7">
         <v>0</v>
@@ -1757,17 +1776,17 @@
         <v>0</v>
       </c>
       <c r="T7">
+        <v>0</v>
+      </c>
+      <c r="U7">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="U7">
-        <v>10</v>
-      </c>
       <c r="V7">
         <v>10</v>
       </c>
       <c r="W7">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="X7">
         <v>0</v>
@@ -1779,18 +1798,18 @@
         <v>0</v>
       </c>
       <c r="AA7">
+        <v>0</v>
+      </c>
+      <c r="AB7">
         <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
-      <c r="AB7">
-        <v>15</v>
-      </c>
       <c r="AC7">
+        <v>15</v>
+      </c>
+      <c r="AD7">
         <v>9</v>
       </c>
-      <c r="AD7">
-        <v>0</v>
-      </c>
       <c r="AE7">
         <v>0</v>
       </c>
@@ -1801,11 +1820,14 @@
         <v>0</v>
       </c>
       <c r="AH7">
+        <v>0</v>
+      </c>
+      <c r="AI7">
         <f t="shared" si="2"/>
         <v>0.375</v>
       </c>
     </row>
-    <row r="8" spans="1:34">
+    <row r="8" spans="1:35">
       <c r="A8">
         <v>1005</v>
       </c>
@@ -1813,51 +1835,51 @@
         <v>4</v>
       </c>
       <c r="C8">
-        <v>20</v>
+        <v>1.55</v>
       </c>
       <c r="D8">
+        <v>20</v>
+      </c>
+      <c r="E8">
         <v>48</v>
       </c>
-      <c r="E8">
+      <c r="F8">
         <v>18</v>
       </c>
-      <c r="F8">
+      <c r="G8">
         <v>36</v>
       </c>
-      <c r="G8">
-        <v>10</v>
-      </c>
       <c r="H8">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="I8">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="J8">
+        <v>10</v>
+      </c>
+      <c r="K8">
         <v>5</v>
       </c>
-      <c r="K8">
-        <v>0</v>
-      </c>
       <c r="L8">
         <v>0</v>
       </c>
       <c r="M8">
+        <v>0</v>
+      </c>
+      <c r="N8">
         <f t="shared" si="3"/>
         <v>1.25</v>
       </c>
-      <c r="N8">
-        <v>15</v>
-      </c>
       <c r="O8">
         <v>15</v>
       </c>
       <c r="P8">
+        <v>15</v>
+      </c>
+      <c r="Q8">
         <v>5</v>
       </c>
-      <c r="Q8">
-        <v>0</v>
-      </c>
       <c r="R8">
         <v>0</v>
       </c>
@@ -1865,21 +1887,21 @@
         <v>0</v>
       </c>
       <c r="T8">
+        <v>0</v>
+      </c>
+      <c r="U8">
         <f t="shared" si="0"/>
         <v>0.714285714285714</v>
       </c>
-      <c r="U8">
-        <v>10</v>
-      </c>
       <c r="V8">
         <v>10</v>
       </c>
       <c r="W8">
+        <v>10</v>
+      </c>
+      <c r="X8">
         <v>5</v>
       </c>
-      <c r="X8">
-        <v>0</v>
-      </c>
       <c r="Y8">
         <v>0</v>
       </c>
@@ -1887,18 +1909,18 @@
         <v>0</v>
       </c>
       <c r="AA8">
+        <v>0</v>
+      </c>
+      <c r="AB8">
         <f t="shared" si="1"/>
         <v>0.8</v>
       </c>
-      <c r="AB8">
-        <v>15</v>
-      </c>
       <c r="AC8">
+        <v>15</v>
+      </c>
+      <c r="AD8">
         <v>12</v>
       </c>
-      <c r="AD8">
-        <v>0</v>
-      </c>
       <c r="AE8">
         <v>0</v>
       </c>
@@ -1909,11 +1931,14 @@
         <v>0</v>
       </c>
       <c r="AH8">
+        <v>0</v>
+      </c>
+      <c r="AI8">
         <f t="shared" si="2"/>
         <v>0.444444444444444</v>
       </c>
     </row>
-    <row r="9" spans="1:34">
+    <row r="9" spans="1:35">
       <c r="A9">
         <v>1006</v>
       </c>
@@ -1921,50 +1946,50 @@
         <v>5</v>
       </c>
       <c r="C9">
-        <v>20</v>
+        <v>1.55</v>
       </c>
       <c r="D9">
+        <v>20</v>
+      </c>
+      <c r="E9">
         <v>47</v>
       </c>
-      <c r="E9">
+      <c r="F9">
         <v>18</v>
       </c>
-      <c r="F9">
+      <c r="G9">
         <v>35</v>
       </c>
-      <c r="G9">
-        <v>10</v>
-      </c>
       <c r="H9">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="I9">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="J9">
         <v>10</v>
       </c>
       <c r="K9">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="L9">
         <v>0</v>
       </c>
       <c r="M9">
+        <v>0</v>
+      </c>
+      <c r="N9">
         <f t="shared" si="3"/>
         <v>1.44444444444444</v>
       </c>
-      <c r="N9">
-        <v>15</v>
-      </c>
       <c r="O9">
         <v>15</v>
       </c>
       <c r="P9">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="Q9">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="R9">
         <v>0</v>
@@ -1973,20 +1998,20 @@
         <v>0</v>
       </c>
       <c r="T9">
+        <v>0</v>
+      </c>
+      <c r="U9">
         <f t="shared" si="0"/>
         <v>0.875</v>
       </c>
-      <c r="U9">
-        <v>10</v>
-      </c>
       <c r="V9">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="W9">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="X9">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="Y9">
         <v>0</v>
@@ -1995,17 +2020,17 @@
         <v>0</v>
       </c>
       <c r="AA9">
+        <v>0</v>
+      </c>
+      <c r="AB9">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="AB9">
-        <v>15</v>
-      </c>
       <c r="AC9">
         <v>15</v>
       </c>
       <c r="AD9">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="AE9">
         <v>0</v>
@@ -2017,11 +2042,14 @@
         <v>0</v>
       </c>
       <c r="AH9">
+        <v>0</v>
+      </c>
+      <c r="AI9">
         <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
     </row>
-    <row r="10" spans="1:34">
+    <row r="10" spans="1:35">
       <c r="A10">
         <v>1007</v>
       </c>
@@ -2029,42 +2057,42 @@
         <v>6</v>
       </c>
       <c r="C10">
+        <v>1.55</v>
+      </c>
+      <c r="D10">
         <v>21</v>
       </c>
-      <c r="D10">
+      <c r="E10">
         <v>47</v>
       </c>
-      <c r="E10">
+      <c r="F10">
         <v>18</v>
       </c>
-      <c r="F10">
+      <c r="G10">
         <v>35</v>
       </c>
-      <c r="G10">
+      <c r="H10">
         <v>5</v>
       </c>
-      <c r="H10">
-        <v>15</v>
-      </c>
       <c r="I10">
         <v>15</v>
       </c>
       <c r="J10">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="K10">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="L10">
         <v>0</v>
       </c>
       <c r="M10">
+        <v>0</v>
+      </c>
+      <c r="N10">
         <f t="shared" si="3"/>
         <v>1.66666666666667</v>
       </c>
-      <c r="N10">
-        <v>15</v>
-      </c>
       <c r="O10">
         <v>15</v>
       </c>
@@ -2072,7 +2100,7 @@
         <v>15</v>
       </c>
       <c r="Q10">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="R10">
         <v>0</v>
@@ -2081,43 +2109,43 @@
         <v>0</v>
       </c>
       <c r="T10">
+        <v>0</v>
+      </c>
+      <c r="U10">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="U10">
-        <v>10</v>
-      </c>
       <c r="V10">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="W10">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="X10">
+        <v>10</v>
+      </c>
+      <c r="Y10">
         <v>5</v>
       </c>
-      <c r="Y10">
-        <v>0</v>
-      </c>
       <c r="Z10">
         <v>0</v>
       </c>
       <c r="AA10">
+        <v>0</v>
+      </c>
+      <c r="AB10">
         <f t="shared" si="1"/>
         <v>1.25</v>
       </c>
-      <c r="AB10">
-        <v>15</v>
-      </c>
       <c r="AC10">
         <v>15</v>
       </c>
       <c r="AD10">
+        <v>15</v>
+      </c>
+      <c r="AE10">
         <v>3</v>
       </c>
-      <c r="AE10">
-        <v>0</v>
-      </c>
       <c r="AF10">
         <v>0</v>
       </c>
@@ -2125,11 +2153,14 @@
         <v>0</v>
       </c>
       <c r="AH10">
+        <v>0</v>
+      </c>
+      <c r="AI10">
         <f t="shared" si="2"/>
         <v>0.636363636363636</v>
       </c>
     </row>
-    <row r="11" spans="1:34">
+    <row r="11" spans="1:35">
       <c r="A11">
         <v>1008</v>
       </c>
@@ -2137,42 +2168,42 @@
         <v>7</v>
       </c>
       <c r="C11">
+        <v>1.55</v>
+      </c>
+      <c r="D11">
         <v>21</v>
       </c>
-      <c r="D11">
+      <c r="E11">
         <v>46</v>
       </c>
-      <c r="E11">
+      <c r="F11">
         <v>18</v>
       </c>
-      <c r="F11">
+      <c r="G11">
         <v>34</v>
       </c>
-      <c r="G11">
+      <c r="H11">
         <v>5</v>
       </c>
-      <c r="H11">
-        <v>15</v>
-      </c>
       <c r="I11">
         <v>15</v>
       </c>
       <c r="J11">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="K11">
+        <v>10</v>
+      </c>
+      <c r="L11">
         <v>5</v>
       </c>
-      <c r="L11">
-        <v>0</v>
-      </c>
       <c r="M11">
+        <v>0</v>
+      </c>
+      <c r="N11">
         <f t="shared" si="3"/>
         <v>1.9</v>
       </c>
-      <c r="N11">
-        <v>15</v>
-      </c>
       <c r="O11">
         <v>15</v>
       </c>
@@ -2180,52 +2211,52 @@
         <v>15</v>
       </c>
       <c r="Q11">
+        <v>15</v>
+      </c>
+      <c r="R11">
         <v>5</v>
       </c>
-      <c r="R11">
-        <v>0</v>
-      </c>
       <c r="S11">
         <v>0</v>
       </c>
       <c r="T11">
+        <v>0</v>
+      </c>
+      <c r="U11">
         <f t="shared" si="0"/>
         <v>1.2</v>
       </c>
-      <c r="U11">
-        <v>10</v>
-      </c>
       <c r="V11">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="W11">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="X11">
         <v>10</v>
       </c>
       <c r="Y11">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="Z11">
         <v>0</v>
       </c>
       <c r="AA11">
+        <v>0</v>
+      </c>
+      <c r="AB11">
         <f t="shared" si="1"/>
         <v>1.44444444444444</v>
       </c>
-      <c r="AB11">
-        <v>15</v>
-      </c>
       <c r="AC11">
         <v>15</v>
       </c>
       <c r="AD11">
+        <v>15</v>
+      </c>
+      <c r="AE11">
         <v>6</v>
       </c>
-      <c r="AE11">
-        <v>0</v>
-      </c>
       <c r="AF11">
         <v>0</v>
       </c>
@@ -2233,11 +2264,14 @@
         <v>0</v>
       </c>
       <c r="AH11">
+        <v>0</v>
+      </c>
+      <c r="AI11">
         <f t="shared" si="2"/>
         <v>0.75</v>
       </c>
     </row>
-    <row r="12" spans="1:34">
+    <row r="12" spans="1:35">
       <c r="A12">
         <v>1009</v>
       </c>
@@ -2245,42 +2279,42 @@
         <v>8</v>
       </c>
       <c r="C12">
+        <v>1.55</v>
+      </c>
+      <c r="D12">
         <v>22</v>
       </c>
-      <c r="D12">
+      <c r="E12">
         <v>46</v>
       </c>
-      <c r="E12">
+      <c r="F12">
         <v>18</v>
       </c>
-      <c r="F12">
+      <c r="G12">
         <v>34</v>
       </c>
-      <c r="G12">
+      <c r="H12">
         <v>5</v>
       </c>
-      <c r="H12">
-        <v>15</v>
-      </c>
       <c r="I12">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="J12">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="K12">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="L12">
+        <v>10</v>
+      </c>
+      <c r="M12">
         <v>5</v>
       </c>
-      <c r="M12">
+      <c r="N12">
         <f t="shared" si="3"/>
         <v>2.35714285714286</v>
       </c>
-      <c r="N12">
-        <v>15</v>
-      </c>
       <c r="O12">
         <v>15</v>
       </c>
@@ -2288,52 +2322,52 @@
         <v>15</v>
       </c>
       <c r="Q12">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="R12">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="S12">
         <v>0</v>
       </c>
       <c r="T12">
+        <v>0</v>
+      </c>
+      <c r="U12">
         <f t="shared" si="0"/>
         <v>1.36363636363636</v>
       </c>
-      <c r="U12">
+      <c r="V12">
         <v>5</v>
       </c>
-      <c r="V12">
-        <v>15</v>
-      </c>
       <c r="W12">
         <v>15</v>
       </c>
       <c r="X12">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="Y12">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="Z12">
         <v>0</v>
       </c>
       <c r="AA12">
+        <v>0</v>
+      </c>
+      <c r="AB12">
         <f t="shared" si="1"/>
         <v>1.66666666666667</v>
       </c>
-      <c r="AB12">
-        <v>15</v>
-      </c>
       <c r="AC12">
         <v>15</v>
       </c>
       <c r="AD12">
+        <v>15</v>
+      </c>
+      <c r="AE12">
         <v>9</v>
       </c>
-      <c r="AE12">
-        <v>0</v>
-      </c>
       <c r="AF12">
         <v>0</v>
       </c>
@@ -2341,11 +2375,14 @@
         <v>0</v>
       </c>
       <c r="AH12">
+        <v>0</v>
+      </c>
+      <c r="AI12">
         <f t="shared" si="2"/>
         <v>0.846153846153846</v>
       </c>
     </row>
-    <row r="13" spans="1:34">
+    <row r="13" spans="1:35">
       <c r="A13">
         <v>1010</v>
       </c>
@@ -2353,42 +2390,42 @@
         <v>9</v>
       </c>
       <c r="C13">
+        <v>1.55</v>
+      </c>
+      <c r="D13">
         <v>22</v>
       </c>
-      <c r="D13">
+      <c r="E13">
         <v>45</v>
       </c>
-      <c r="E13">
+      <c r="F13">
         <v>18</v>
       </c>
-      <c r="F13">
+      <c r="G13">
         <v>33</v>
       </c>
-      <c r="G13">
+      <c r="H13">
         <v>3</v>
       </c>
-      <c r="H13">
-        <v>15</v>
-      </c>
       <c r="I13">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="J13">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="K13">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="L13">
+        <v>10</v>
+      </c>
+      <c r="M13">
         <v>5</v>
       </c>
-      <c r="M13">
+      <c r="N13">
         <f t="shared" si="3"/>
         <v>2.42647058823529</v>
       </c>
-      <c r="N13">
-        <v>15</v>
-      </c>
       <c r="O13">
         <v>15</v>
       </c>
@@ -2399,49 +2436,49 @@
         <v>15</v>
       </c>
       <c r="R13">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="S13">
         <v>0</v>
       </c>
       <c r="T13">
+        <v>0</v>
+      </c>
+      <c r="U13">
         <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
-      <c r="U13">
+      <c r="V13">
         <v>5</v>
       </c>
-      <c r="V13">
-        <v>15</v>
-      </c>
       <c r="W13">
         <v>15</v>
       </c>
       <c r="X13">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="Y13">
+        <v>10</v>
+      </c>
+      <c r="Z13">
         <v>5</v>
       </c>
-      <c r="Z13">
-        <v>0</v>
-      </c>
       <c r="AA13">
+        <v>0</v>
+      </c>
+      <c r="AB13">
         <f t="shared" si="1"/>
         <v>1.9</v>
       </c>
-      <c r="AB13">
-        <v>15</v>
-      </c>
       <c r="AC13">
         <v>15</v>
       </c>
       <c r="AD13">
+        <v>15</v>
+      </c>
+      <c r="AE13">
         <v>12</v>
       </c>
-      <c r="AE13">
-        <v>0</v>
-      </c>
       <c r="AF13">
         <v>0</v>
       </c>
@@ -2449,11 +2486,14 @@
         <v>0</v>
       </c>
       <c r="AH13">
+        <v>0</v>
+      </c>
+      <c r="AI13">
         <f t="shared" si="2"/>
         <v>0.928571428571429</v>
       </c>
     </row>
-    <row r="14" spans="1:34">
+    <row r="14" spans="1:35">
       <c r="A14">
         <v>1011</v>
       </c>
@@ -2461,86 +2501,86 @@
         <v>10</v>
       </c>
       <c r="C14">
+        <v>1.5</v>
+      </c>
+      <c r="D14">
         <v>23</v>
       </c>
-      <c r="D14">
+      <c r="E14">
         <v>45</v>
       </c>
-      <c r="E14">
+      <c r="F14">
         <v>18</v>
       </c>
-      <c r="F14">
+      <c r="G14">
         <v>33</v>
       </c>
-      <c r="G14">
+      <c r="H14">
         <v>3</v>
       </c>
-      <c r="H14">
-        <v>10</v>
-      </c>
       <c r="I14">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="J14">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="K14">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="L14">
+        <v>10</v>
+      </c>
+      <c r="M14">
         <v>5</v>
       </c>
-      <c r="M14">
+      <c r="N14">
         <f t="shared" si="3"/>
         <v>2.53968253968254</v>
       </c>
-      <c r="N14">
-        <v>15</v>
-      </c>
       <c r="O14">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="P14">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="Q14">
         <v>15</v>
       </c>
       <c r="R14">
+        <v>15</v>
+      </c>
+      <c r="S14">
         <v>5</v>
       </c>
-      <c r="S14">
-        <v>0</v>
-      </c>
       <c r="T14">
+        <v>0</v>
+      </c>
+      <c r="U14">
         <f t="shared" si="0"/>
         <v>1.64285714285714</v>
       </c>
-      <c r="U14">
+      <c r="V14">
         <v>5</v>
       </c>
-      <c r="V14">
-        <v>15</v>
-      </c>
       <c r="W14">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="X14">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="Y14">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="Z14">
+        <v>10</v>
+      </c>
+      <c r="AA14">
         <v>5</v>
       </c>
-      <c r="AA14">
+      <c r="AB14">
         <f t="shared" si="1"/>
         <v>2.35714285714286</v>
       </c>
-      <c r="AB14">
-        <v>15</v>
-      </c>
       <c r="AC14">
         <v>15</v>
       </c>
@@ -2548,7 +2588,7 @@
         <v>15</v>
       </c>
       <c r="AE14">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="AF14">
         <v>0</v>
@@ -2557,11 +2597,14 @@
         <v>0</v>
       </c>
       <c r="AH14">
+        <v>0</v>
+      </c>
+      <c r="AI14">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:34">
+    <row r="15" spans="1:35">
       <c r="A15">
         <v>1012</v>
       </c>
@@ -2569,44 +2612,44 @@
         <v>12</v>
       </c>
       <c r="C15">
+        <v>1.5</v>
+      </c>
+      <c r="D15">
         <v>23</v>
       </c>
-      <c r="D15">
+      <c r="E15">
         <v>44</v>
       </c>
-      <c r="E15">
+      <c r="F15">
         <v>18</v>
       </c>
-      <c r="F15">
+      <c r="G15">
         <v>32</v>
       </c>
-      <c r="G15">
+      <c r="H15">
         <v>2</v>
       </c>
-      <c r="H15">
-        <v>10</v>
-      </c>
       <c r="I15">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="J15">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="K15">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="L15">
         <v>10</v>
       </c>
       <c r="M15">
+        <v>10</v>
+      </c>
+      <c r="N15">
         <f t="shared" si="3"/>
         <v>2.76119402985075</v>
       </c>
-      <c r="N15">
-        <v>15</v>
-      </c>
       <c r="O15">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="P15">
         <v>20</v>
@@ -2615,40 +2658,40 @@
         <v>20</v>
       </c>
       <c r="R15">
+        <v>20</v>
+      </c>
+      <c r="S15">
         <v>5</v>
       </c>
-      <c r="S15">
-        <v>0</v>
-      </c>
       <c r="T15">
+        <v>0</v>
+      </c>
+      <c r="U15">
         <f t="shared" si="0"/>
         <v>1.75</v>
       </c>
-      <c r="U15">
+      <c r="V15">
         <v>3</v>
       </c>
-      <c r="V15">
-        <v>15</v>
-      </c>
       <c r="W15">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="X15">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="Y15">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="Z15">
+        <v>10</v>
+      </c>
+      <c r="AA15">
         <v>5</v>
       </c>
-      <c r="AA15">
+      <c r="AB15">
         <f t="shared" si="1"/>
         <v>2.42647058823529</v>
       </c>
-      <c r="AB15">
-        <v>15</v>
-      </c>
       <c r="AC15">
         <v>15</v>
       </c>
@@ -2656,20 +2699,23 @@
         <v>15</v>
       </c>
       <c r="AE15">
+        <v>15</v>
+      </c>
+      <c r="AF15">
         <v>3</v>
       </c>
-      <c r="AF15">
-        <v>0</v>
-      </c>
       <c r="AG15">
         <v>0</v>
       </c>
       <c r="AH15">
+        <v>0</v>
+      </c>
+      <c r="AI15">
         <f t="shared" si="2"/>
         <v>1.125</v>
       </c>
     </row>
-    <row r="16" spans="1:34">
+    <row r="16" spans="1:35">
       <c r="A16">
         <v>1013</v>
       </c>
@@ -2677,44 +2723,44 @@
         <v>14</v>
       </c>
       <c r="C16">
+        <v>1.5</v>
+      </c>
+      <c r="D16">
         <v>24</v>
       </c>
-      <c r="D16">
+      <c r="E16">
         <v>44</v>
       </c>
-      <c r="E16">
+      <c r="F16">
         <v>18</v>
       </c>
-      <c r="F16">
+      <c r="G16">
         <v>32</v>
       </c>
-      <c r="G16">
+      <c r="H16">
         <v>2</v>
       </c>
-      <c r="H16">
-        <v>10</v>
-      </c>
       <c r="I16">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="J16">
         <v>20</v>
       </c>
       <c r="K16">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="L16">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="M16">
+        <v>10</v>
+      </c>
+      <c r="N16">
         <f t="shared" si="3"/>
         <v>2.85714285714286</v>
       </c>
-      <c r="N16">
-        <v>15</v>
-      </c>
       <c r="O16">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="P16">
         <v>20</v>
@@ -2723,40 +2769,40 @@
         <v>20</v>
       </c>
       <c r="R16">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="S16">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="T16">
+        <v>0</v>
+      </c>
+      <c r="U16">
         <f t="shared" si="0"/>
         <v>1.88235294117647</v>
       </c>
-      <c r="U16">
+      <c r="V16">
         <v>3</v>
       </c>
-      <c r="V16">
-        <v>10</v>
-      </c>
       <c r="W16">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="X16">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="Y16">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="Z16">
+        <v>10</v>
+      </c>
+      <c r="AA16">
         <v>5</v>
       </c>
-      <c r="AA16">
+      <c r="AB16">
         <f t="shared" si="1"/>
         <v>2.53968253968254</v>
       </c>
-      <c r="AB16">
-        <v>15</v>
-      </c>
       <c r="AC16">
         <v>15</v>
       </c>
@@ -2764,20 +2810,23 @@
         <v>15</v>
       </c>
       <c r="AE16">
+        <v>15</v>
+      </c>
+      <c r="AF16">
         <v>6</v>
       </c>
-      <c r="AF16">
-        <v>0</v>
-      </c>
       <c r="AG16">
         <v>0</v>
       </c>
       <c r="AH16">
+        <v>0</v>
+      </c>
+      <c r="AI16">
         <f t="shared" si="2"/>
         <v>1.23529411764706</v>
       </c>
     </row>
-    <row r="17" spans="1:34">
+    <row r="17" spans="1:35">
       <c r="A17">
         <v>1014</v>
       </c>
@@ -2785,86 +2834,86 @@
         <v>16</v>
       </c>
       <c r="C17">
+        <v>1.5</v>
+      </c>
+      <c r="D17">
         <v>24</v>
       </c>
-      <c r="D17">
+      <c r="E17">
         <v>43</v>
       </c>
-      <c r="E17">
+      <c r="F17">
         <v>18</v>
       </c>
-      <c r="F17">
+      <c r="G17">
         <v>31</v>
       </c>
-      <c r="G17">
+      <c r="H17">
         <v>1</v>
       </c>
-      <c r="H17">
+      <c r="I17">
         <v>5</v>
       </c>
-      <c r="I17">
-        <v>20</v>
-      </c>
       <c r="J17">
+        <v>20</v>
+      </c>
+      <c r="K17">
         <v>25</v>
       </c>
-      <c r="K17">
-        <v>20</v>
-      </c>
       <c r="L17">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="M17">
+        <v>15</v>
+      </c>
+      <c r="N17">
         <f t="shared" si="3"/>
         <v>3.19767441860465</v>
       </c>
-      <c r="N17">
-        <v>15</v>
-      </c>
       <c r="O17">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="P17">
         <v>20</v>
       </c>
       <c r="Q17">
+        <v>20</v>
+      </c>
+      <c r="R17">
         <v>25</v>
       </c>
-      <c r="R17">
-        <v>10</v>
-      </c>
       <c r="S17">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="T17">
+        <v>0</v>
+      </c>
+      <c r="U17">
         <f t="shared" si="0"/>
         <v>1.94444444444444</v>
       </c>
-      <c r="U17">
+      <c r="V17">
         <v>2</v>
       </c>
-      <c r="V17">
-        <v>10</v>
-      </c>
       <c r="W17">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="X17">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="Y17">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="Z17">
         <v>10</v>
       </c>
       <c r="AA17">
+        <v>10</v>
+      </c>
+      <c r="AB17">
         <f t="shared" si="1"/>
         <v>2.76119402985075</v>
       </c>
-      <c r="AB17">
-        <v>15</v>
-      </c>
       <c r="AC17">
         <v>15</v>
       </c>
@@ -2872,20 +2921,23 @@
         <v>15</v>
       </c>
       <c r="AE17">
+        <v>15</v>
+      </c>
+      <c r="AF17">
         <v>9</v>
       </c>
-      <c r="AF17">
-        <v>0</v>
-      </c>
       <c r="AG17">
         <v>0</v>
       </c>
       <c r="AH17">
+        <v>0</v>
+      </c>
+      <c r="AI17">
         <f t="shared" si="2"/>
         <v>1.33333333333333</v>
       </c>
     </row>
-    <row r="18" spans="1:34">
+    <row r="18" spans="1:35">
       <c r="A18">
         <v>1015</v>
       </c>
@@ -2893,86 +2945,86 @@
         <v>18</v>
       </c>
       <c r="C18">
+        <v>1.45</v>
+      </c>
+      <c r="D18">
         <v>25</v>
       </c>
-      <c r="D18">
+      <c r="E18">
         <v>43</v>
       </c>
-      <c r="E18">
+      <c r="F18">
         <v>18</v>
       </c>
-      <c r="F18">
+      <c r="G18">
         <v>31</v>
       </c>
-      <c r="G18">
+      <c r="H18">
         <v>1</v>
       </c>
-      <c r="H18">
+      <c r="I18">
         <v>5</v>
       </c>
-      <c r="I18">
-        <v>20</v>
-      </c>
       <c r="J18">
+        <v>20</v>
+      </c>
+      <c r="K18">
         <v>25</v>
       </c>
-      <c r="K18">
-        <v>20</v>
-      </c>
       <c r="L18">
         <v>20</v>
       </c>
       <c r="M18">
+        <v>20</v>
+      </c>
+      <c r="N18">
         <f t="shared" si="3"/>
         <v>3.2967032967033</v>
       </c>
-      <c r="N18">
-        <v>15</v>
-      </c>
       <c r="O18">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="P18">
         <v>20</v>
       </c>
       <c r="Q18">
+        <v>20</v>
+      </c>
+      <c r="R18">
         <v>30</v>
       </c>
-      <c r="R18">
-        <v>10</v>
-      </c>
       <c r="S18">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="T18">
+        <v>0</v>
+      </c>
+      <c r="U18">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="U18">
+      <c r="V18">
         <v>2</v>
       </c>
-      <c r="V18">
-        <v>10</v>
-      </c>
       <c r="W18">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="X18">
         <v>20</v>
       </c>
       <c r="Y18">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="Z18">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="AA18">
+        <v>10</v>
+      </c>
+      <c r="AB18">
         <f t="shared" si="1"/>
         <v>2.85714285714286</v>
       </c>
-      <c r="AB18">
-        <v>15</v>
-      </c>
       <c r="AC18">
         <v>15</v>
       </c>
@@ -2980,20 +3032,23 @@
         <v>15</v>
       </c>
       <c r="AE18">
+        <v>15</v>
+      </c>
+      <c r="AF18">
         <v>12</v>
       </c>
-      <c r="AF18">
-        <v>0</v>
-      </c>
       <c r="AG18">
         <v>0</v>
       </c>
       <c r="AH18">
+        <v>0</v>
+      </c>
+      <c r="AI18">
         <f t="shared" si="2"/>
         <v>1.42105263157895</v>
       </c>
     </row>
-    <row r="19" spans="1:34">
+    <row r="19" spans="1:35">
       <c r="A19">
         <v>1016</v>
       </c>
@@ -3001,86 +3056,86 @@
         <v>20</v>
       </c>
       <c r="C19">
+        <v>1.45</v>
+      </c>
+      <c r="D19">
         <v>25</v>
       </c>
-      <c r="D19">
+      <c r="E19">
         <v>42</v>
       </c>
-      <c r="E19">
+      <c r="F19">
         <v>18</v>
       </c>
-      <c r="F19">
+      <c r="G19">
         <v>30</v>
       </c>
-      <c r="G19">
+      <c r="H19">
         <v>1</v>
       </c>
-      <c r="H19">
+      <c r="I19">
         <v>3</v>
       </c>
-      <c r="I19">
-        <v>15</v>
-      </c>
       <c r="J19">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="K19">
         <v>25</v>
       </c>
       <c r="L19">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="M19">
+        <v>20</v>
+      </c>
+      <c r="N19">
         <f t="shared" si="3"/>
         <v>3.46067415730337</v>
       </c>
-      <c r="N19">
-        <v>15</v>
-      </c>
       <c r="O19">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="P19">
         <v>20</v>
       </c>
       <c r="Q19">
+        <v>20</v>
+      </c>
+      <c r="R19">
         <v>30</v>
       </c>
-      <c r="R19">
-        <v>15</v>
-      </c>
       <c r="S19">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="T19">
-        <f t="shared" ref="T19:T23" si="4">(N19*0+O19*1+P19*2+Q19*3+R19*4+S19*5)/(N19+O19+P19+Q19+R19+S19)</f>
+        <v>0</v>
+      </c>
+      <c r="U19">
+        <f t="shared" ref="U19:U23" si="4">(O19*0+P19*1+Q19*2+R19*3+S19*4+T19*5)/(O19+P19+Q19+R19+S19+T19)</f>
         <v>2.1</v>
       </c>
-      <c r="U19">
+      <c r="V19">
         <v>1</v>
       </c>
-      <c r="V19">
+      <c r="W19">
         <v>5</v>
       </c>
-      <c r="W19">
-        <v>20</v>
-      </c>
       <c r="X19">
+        <v>20</v>
+      </c>
+      <c r="Y19">
         <v>30</v>
       </c>
-      <c r="Y19">
-        <v>20</v>
-      </c>
       <c r="Z19">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="AA19">
+        <v>10</v>
+      </c>
+      <c r="AB19">
         <f t="shared" si="1"/>
         <v>3.08139534883721</v>
       </c>
-      <c r="AB19">
-        <v>15</v>
-      </c>
       <c r="AC19">
         <v>15</v>
       </c>
@@ -3091,17 +3146,20 @@
         <v>15</v>
       </c>
       <c r="AF19">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="AG19">
         <v>0</v>
       </c>
       <c r="AH19">
+        <v>0</v>
+      </c>
+      <c r="AI19">
         <f t="shared" si="2"/>
         <v>1.5</v>
       </c>
     </row>
-    <row r="20" spans="1:34">
+    <row r="20" spans="1:35">
       <c r="A20">
         <v>1017</v>
       </c>
@@ -3109,28 +3167,28 @@
         <v>22</v>
       </c>
       <c r="C20">
+        <v>1.45</v>
+      </c>
+      <c r="D20">
         <v>26</v>
       </c>
-      <c r="D20">
+      <c r="E20">
         <v>42</v>
       </c>
-      <c r="E20">
+      <c r="F20">
         <v>18</v>
       </c>
-      <c r="F20">
+      <c r="G20">
         <v>30</v>
       </c>
-      <c r="G20">
+      <c r="H20">
         <v>1</v>
       </c>
-      <c r="H20">
+      <c r="I20">
         <v>3</v>
       </c>
-      <c r="I20">
-        <v>15</v>
-      </c>
       <c r="J20">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="K20">
         <v>25</v>
@@ -3139,77 +3197,80 @@
         <v>25</v>
       </c>
       <c r="M20">
+        <v>25</v>
+      </c>
+      <c r="N20">
         <f t="shared" si="3"/>
         <v>3.54255319148936</v>
       </c>
-      <c r="N20">
-        <v>15</v>
-      </c>
       <c r="O20">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="P20">
         <v>20</v>
       </c>
       <c r="Q20">
+        <v>20</v>
+      </c>
+      <c r="R20">
         <v>35</v>
       </c>
-      <c r="R20">
-        <v>15</v>
-      </c>
       <c r="S20">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="T20">
+        <v>0</v>
+      </c>
+      <c r="U20">
         <f t="shared" si="4"/>
         <v>2.14285714285714</v>
       </c>
-      <c r="U20">
+      <c r="V20">
         <v>1</v>
       </c>
-      <c r="V20">
+      <c r="W20">
         <v>4</v>
       </c>
-      <c r="W20">
+      <c r="X20">
         <v>18</v>
       </c>
-      <c r="X20">
+      <c r="Y20">
         <v>30</v>
       </c>
-      <c r="Y20">
-        <v>20</v>
-      </c>
       <c r="Z20">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="AA20">
+        <v>10</v>
+      </c>
+      <c r="AB20">
         <f t="shared" si="1"/>
         <v>3.13253012048193</v>
       </c>
-      <c r="AB20">
-        <v>15</v>
-      </c>
       <c r="AC20">
         <v>15</v>
       </c>
       <c r="AD20">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="AE20">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="AF20">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="AG20">
         <v>0</v>
       </c>
       <c r="AH20">
+        <v>0</v>
+      </c>
+      <c r="AI20">
         <f t="shared" si="2"/>
         <v>1.53846153846154</v>
       </c>
     </row>
-    <row r="21" spans="1:34">
+    <row r="21" spans="1:35">
       <c r="A21">
         <v>1018</v>
       </c>
@@ -3217,28 +3278,28 @@
         <v>24</v>
       </c>
       <c r="C21">
+        <v>1.4</v>
+      </c>
+      <c r="D21">
         <v>26</v>
       </c>
-      <c r="D21">
+      <c r="E21">
         <v>41</v>
       </c>
-      <c r="E21">
+      <c r="F21">
         <v>18</v>
       </c>
-      <c r="F21">
+      <c r="G21">
         <v>29</v>
       </c>
-      <c r="G21">
+      <c r="H21">
         <v>1</v>
       </c>
-      <c r="H21">
+      <c r="I21">
         <v>3</v>
       </c>
-      <c r="I21">
-        <v>10</v>
-      </c>
       <c r="J21">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="K21">
         <v>25</v>
@@ -3247,77 +3308,80 @@
         <v>25</v>
       </c>
       <c r="M21">
+        <v>25</v>
+      </c>
+      <c r="N21">
         <f t="shared" si="3"/>
         <v>3.62921348314607</v>
       </c>
-      <c r="N21">
-        <v>15</v>
-      </c>
       <c r="O21">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="P21">
         <v>20</v>
       </c>
       <c r="Q21">
+        <v>20</v>
+      </c>
+      <c r="R21">
         <v>35</v>
       </c>
-      <c r="R21">
-        <v>20</v>
-      </c>
       <c r="S21">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="T21">
+        <v>0</v>
+      </c>
+      <c r="U21">
         <f t="shared" si="4"/>
         <v>2.22727272727273</v>
       </c>
-      <c r="U21">
+      <c r="V21">
         <v>1</v>
       </c>
-      <c r="V21">
+      <c r="W21">
         <v>3</v>
       </c>
-      <c r="W21">
+      <c r="X21">
         <v>16</v>
       </c>
-      <c r="X21">
+      <c r="Y21">
         <v>30</v>
       </c>
-      <c r="Y21">
-        <v>20</v>
-      </c>
       <c r="Z21">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="AA21">
+        <v>10</v>
+      </c>
+      <c r="AB21">
         <f t="shared" si="1"/>
         <v>3.1875</v>
       </c>
-      <c r="AB21">
-        <v>15</v>
-      </c>
       <c r="AC21">
         <v>15</v>
       </c>
       <c r="AD21">
+        <v>15</v>
+      </c>
+      <c r="AE21">
         <v>25</v>
       </c>
-      <c r="AE21">
-        <v>15</v>
-      </c>
       <c r="AF21">
+        <v>15</v>
+      </c>
+      <c r="AG21">
         <v>2</v>
       </c>
-      <c r="AG21">
-        <v>0</v>
-      </c>
       <c r="AH21">
+        <v>0</v>
+      </c>
+      <c r="AI21">
         <f t="shared" si="2"/>
         <v>1.63888888888889</v>
       </c>
     </row>
-    <row r="22" spans="1:34">
+    <row r="22" spans="1:35">
       <c r="A22">
         <v>1019</v>
       </c>
@@ -3325,107 +3389,110 @@
         <v>26</v>
       </c>
       <c r="C22">
+        <v>1.4</v>
+      </c>
+      <c r="D22">
         <v>27</v>
       </c>
-      <c r="D22">
+      <c r="E22">
         <v>41</v>
       </c>
-      <c r="E22">
+      <c r="F22">
         <v>18</v>
       </c>
-      <c r="F22">
+      <c r="G22">
         <v>29</v>
-      </c>
-      <c r="G22">
-        <v>1</v>
       </c>
       <c r="H22">
         <v>1</v>
       </c>
       <c r="I22">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="J22">
+        <v>10</v>
+      </c>
+      <c r="K22">
         <v>25</v>
       </c>
-      <c r="K22">
+      <c r="L22">
         <v>40</v>
       </c>
-      <c r="L22">
+      <c r="M22">
         <v>25</v>
       </c>
-      <c r="M22">
+      <c r="N22">
         <f t="shared" si="3"/>
         <v>3.73529411764706</v>
       </c>
-      <c r="N22">
-        <v>15</v>
-      </c>
       <c r="O22">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="P22">
         <v>20</v>
       </c>
       <c r="Q22">
+        <v>20</v>
+      </c>
+      <c r="R22">
         <v>45</v>
       </c>
-      <c r="R22">
+      <c r="S22">
         <v>22</v>
       </c>
-      <c r="S22">
-        <v>0</v>
-      </c>
       <c r="T22">
+        <v>0</v>
+      </c>
+      <c r="U22">
         <f t="shared" si="4"/>
         <v>2.31967213114754</v>
       </c>
-      <c r="U22">
+      <c r="V22">
         <v>1</v>
       </c>
-      <c r="V22">
+      <c r="W22">
         <v>2</v>
       </c>
-      <c r="W22">
+      <c r="X22">
         <v>14</v>
       </c>
-      <c r="X22">
+      <c r="Y22">
         <v>30</v>
       </c>
-      <c r="Y22">
-        <v>20</v>
-      </c>
       <c r="Z22">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="AA22">
+        <v>10</v>
+      </c>
+      <c r="AB22">
         <f t="shared" si="1"/>
         <v>3.24675324675325</v>
       </c>
-      <c r="AB22">
-        <v>15</v>
-      </c>
       <c r="AC22">
         <v>15</v>
       </c>
       <c r="AD22">
+        <v>15</v>
+      </c>
+      <c r="AE22">
         <v>35</v>
       </c>
-      <c r="AE22">
-        <v>15</v>
-      </c>
       <c r="AF22">
+        <v>15</v>
+      </c>
+      <c r="AG22">
         <v>4</v>
       </c>
-      <c r="AG22">
-        <v>0</v>
-      </c>
       <c r="AH22">
+        <v>0</v>
+      </c>
+      <c r="AI22">
         <f t="shared" si="2"/>
         <v>1.73809523809524</v>
       </c>
     </row>
-    <row r="23" spans="1:34">
+    <row r="23" spans="1:35">
       <c r="A23">
         <v>1020</v>
       </c>
@@ -3433,102 +3500,105 @@
         <v>28</v>
       </c>
       <c r="C23">
+        <v>1.35</v>
+      </c>
+      <c r="D23">
         <v>27</v>
       </c>
-      <c r="D23">
+      <c r="E23">
         <v>40</v>
       </c>
-      <c r="E23">
+      <c r="F23">
         <v>18</v>
       </c>
-      <c r="F23">
+      <c r="G23">
         <v>28</v>
-      </c>
-      <c r="G23">
-        <v>1</v>
       </c>
       <c r="H23">
         <v>1</v>
       </c>
       <c r="I23">
+        <v>1</v>
+      </c>
+      <c r="J23">
         <v>5</v>
       </c>
-      <c r="J23">
+      <c r="K23">
         <v>25</v>
       </c>
-      <c r="K23">
+      <c r="L23">
         <v>40</v>
       </c>
-      <c r="L23">
+      <c r="M23">
         <v>25</v>
       </c>
-      <c r="M23">
+      <c r="N23">
         <f t="shared" si="3"/>
         <v>3.82474226804124</v>
       </c>
-      <c r="N23">
-        <v>15</v>
-      </c>
       <c r="O23">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="P23">
         <v>20</v>
       </c>
       <c r="Q23">
+        <v>20</v>
+      </c>
+      <c r="R23">
         <v>55</v>
       </c>
-      <c r="R23">
+      <c r="S23">
         <v>25</v>
       </c>
-      <c r="S23">
-        <v>0</v>
-      </c>
       <c r="T23">
+        <v>0</v>
+      </c>
+      <c r="U23">
         <f t="shared" si="4"/>
         <v>2.40740740740741</v>
       </c>
-      <c r="U23">
-        <v>1</v>
-      </c>
       <c r="V23">
         <v>1</v>
       </c>
       <c r="W23">
+        <v>1</v>
+      </c>
+      <c r="X23">
         <v>12</v>
       </c>
-      <c r="X23">
+      <c r="Y23">
         <v>30</v>
       </c>
-      <c r="Y23">
-        <v>20</v>
-      </c>
       <c r="Z23">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="AA23">
+        <v>10</v>
+      </c>
+      <c r="AB23">
         <f t="shared" si="1"/>
         <v>3.31081081081081</v>
       </c>
-      <c r="AB23">
-        <v>15</v>
-      </c>
       <c r="AC23">
         <v>15</v>
       </c>
       <c r="AD23">
+        <v>15</v>
+      </c>
+      <c r="AE23">
         <v>45</v>
       </c>
-      <c r="AE23">
-        <v>20</v>
-      </c>
       <c r="AF23">
+        <v>20</v>
+      </c>
+      <c r="AG23">
         <v>5</v>
       </c>
-      <c r="AG23">
-        <v>0</v>
-      </c>
       <c r="AH23">
+        <v>0</v>
+      </c>
+      <c r="AI23">
         <f t="shared" si="2"/>
         <v>1.85</v>
       </c>

</xml_diff>